<commit_message>
fix some issues from refactorization and changes on datatypes
</commit_message>
<xml_diff>
--- a/ExcelGateway/bin/Debug/Book1.xlsx
+++ b/ExcelGateway/bin/Debug/Book1.xlsx
@@ -2,21 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R3189644c069f4ab1"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rf4083c44b0c3412a"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="" visibility="1" width="437" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R0f5c66a60dd54437"/>
+  <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R10ace39b7df04a13"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{c03551ee-a0ef-463b-8f21-08b8ba926a86}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{5ef51013-75bf-44b8-a5cf-73e855c4446d}">
   <we:reference id="c2fcd407-2a85-471d-9a88-692470072d6c" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>